<commit_message>
adding data cut from main set due to missing obs
</commit_message>
<xml_diff>
--- a/data/spore counts incomplete data.xlsx
+++ b/data/spore counts incomplete data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ifmiller/Documents/GitHub/flax.rust/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A5018F8-5806-E64C-90C1-7187EE80CF9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAAA198-91FE-744C-93F2-7D1920F23BA6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="4480" windowWidth="27640" windowHeight="15780" xr2:uid="{5B1D0C83-39A0-B840-8D28-BAB1CF5E45B4}"/>
+    <workbookView xWindow="260" yWindow="960" windowWidth="27640" windowHeight="15780" xr2:uid="{5B1D0C83-39A0-B840-8D28-BAB1CF5E45B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>?</t>
   </si>
@@ -64,16 +64,41 @@
   </si>
   <si>
     <t>unknown direction + distance</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Date deployed</t>
+  </si>
+  <si>
+    <t>no within host data recorded on deploy date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,9 +124,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,15 +443,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37854EFB-BF03-2B43-B5B9-997459A2AFAB}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I4" sqref="I4:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -432,97 +459,400 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44153</v>
       </c>
       <c r="B2">
         <v>262</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>44027</v>
       </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>80</v>
+      <c r="F2" t="s">
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="C14" s="1"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B3" s="3">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44018</v>
+      </c>
+      <c r="D3" s="2">
+        <v>44025</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>80</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B4" s="3">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44018</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44025</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>80</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B5" s="3">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2">
+        <v>44018</v>
+      </c>
+      <c r="D5" s="2">
+        <v>44025</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>80</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B6" s="3">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44018</v>
+      </c>
+      <c r="D6" s="2">
+        <v>44025</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>80</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B7" s="3">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44018</v>
+      </c>
+      <c r="D7" s="2">
+        <v>44025</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3">
+        <v>25</v>
+      </c>
+      <c r="G7" s="3">
+        <v>80</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B8" s="3">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44018</v>
+      </c>
+      <c r="D8" s="2">
+        <v>44025</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3">
+        <v>25</v>
+      </c>
+      <c r="G8" s="3">
+        <v>80</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B9" s="3">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2">
+        <v>44018</v>
+      </c>
+      <c r="D9" s="2">
+        <v>44025</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="3">
+        <v>25</v>
+      </c>
+      <c r="G9" s="3">
+        <v>80</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B10" s="3">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44018</v>
+      </c>
+      <c r="D10" s="2">
+        <v>44025</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3">
+        <v>25</v>
+      </c>
+      <c r="G10" s="3">
+        <v>80</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B11" s="3">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44018</v>
+      </c>
+      <c r="D11" s="2">
+        <v>44025</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="3">
+        <v>50</v>
+      </c>
+      <c r="G11" s="3">
+        <v>80</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B12" s="3">
+        <v>36</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44018</v>
+      </c>
+      <c r="D12" s="2">
+        <v>44025</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="3">
+        <v>50</v>
+      </c>
+      <c r="G12" s="3">
+        <v>80</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B13" s="3">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44018</v>
+      </c>
+      <c r="D13" s="2">
+        <v>44025</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="3">
+        <v>50</v>
+      </c>
+      <c r="G13" s="3">
+        <v>80</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>44125</v>
+      </c>
+      <c r="B14" s="3">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44018</v>
+      </c>
+      <c r="D14" s="2">
+        <v>44025</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="3">
+        <v>50</v>
+      </c>
+      <c r="G14" s="3">
+        <v>80</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>